<commit_message>
Update DbSeeder to improve project code seeding with isActive status
- Enhanced the project code seeding process by integrating the isActive status, allowing for a more accurate representation of project codes.
- Refined data retrieval methods to accommodate the new isActive parameter, increasing the flexibility and effectiveness of the seeding logic.
</commit_message>
<xml_diff>
--- a/CNCToolingDatabase/Data/PROJECT CODE MASTER.xlsx
+++ b/CNCToolingDatabase/Data/PROJECT CODE MASTER.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Public\Documents\Tool-Master-Control\Tool-Master-Control\CNCToolingDatabase\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{314F3389-5208-46DA-BA15-6C72A245F7F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD190ED8-FF37-4028-9E99-94176DB13646}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{8271D9D6-2065-419F-AC52-7850B71D4074}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="115">
   <si>
     <t>No.</t>
   </si>
@@ -376,6 +376,9 @@
   </si>
   <si>
     <t>INACTIVE</t>
+  </si>
+  <si>
+    <t>SAMQQQQ</t>
   </si>
 </sst>
 </file>
@@ -446,16 +449,16 @@
   <dxfs count="7">
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
           <bgColor auto="1"/>
         </patternFill>
       </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -549,8 +552,8 @@
     <tableColumn id="1" xr3:uid="{4A87BED8-B1B5-45DE-BB4C-8C3E6116591E}" name="No." dataDxfId="4"/>
     <tableColumn id="6" xr3:uid="{5E55A1C0-5160-4819-9AC4-BFE97197F01A}" name="Project Code" dataDxfId="3"/>
     <tableColumn id="2" xr3:uid="{E05168FF-5C3E-4D5A-B93D-D4D10BF8E5D9}" name="Customer" dataDxfId="2"/>
-    <tableColumn id="4" xr3:uid="{1036F03E-651A-430D-95B8-23A69E3389A8}" name="Project" dataDxfId="0"/>
-    <tableColumn id="3" xr3:uid="{F3A2A34E-F6A4-4E74-965D-DE476ADF2610}" name="Status" dataDxfId="1"/>
+    <tableColumn id="4" xr3:uid="{1036F03E-651A-430D-95B8-23A69E3389A8}" name="Project" dataDxfId="1"/>
+    <tableColumn id="3" xr3:uid="{F3A2A34E-F6A4-4E74-965D-DE476ADF2610}" name="Status" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -856,7 +859,7 @@
   <dimension ref="A1:E47"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -893,7 +896,7 @@
         <v>4</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>5</v>
+        <v>114</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>6</v>

</xml_diff>

<commit_message>
Refactor DbSeeder to enhance machine model loading and seeding logic
- Updated the DbSeeder to dynamically load machine models from "MACHINE MODEL MASTER.xlsx", improving maintainability and flexibility.
- Incorporated an isActive status for machine models in the seeding process, allowing for a more accurate representation of their activity state.
</commit_message>
<xml_diff>
--- a/CNCToolingDatabase/Data/PROJECT CODE MASTER.xlsx
+++ b/CNCToolingDatabase/Data/PROJECT CODE MASTER.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Public\Documents\Tool-Master-Control\Tool-Master-Control\CNCToolingDatabase\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD190ED8-FF37-4028-9E99-94176DB13646}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFD5A458-7372-4C38-8F61-E2437FE87A88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{8271D9D6-2065-419F-AC52-7850B71D4074}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="114">
   <si>
     <t>No.</t>
   </si>
@@ -376,9 +376,6 @@
   </si>
   <si>
     <t>INACTIVE</t>
-  </si>
-  <si>
-    <t>SAMQQQQ</t>
   </si>
 </sst>
 </file>
@@ -859,7 +856,7 @@
   <dimension ref="A1:E47"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -896,7 +893,7 @@
         <v>4</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>114</v>
+        <v>5</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>6</v>

</xml_diff>